<commit_message>
Updated gerbers for including wireless coil circuit
</commit_message>
<xml_diff>
--- a/kicad/robot/nextPCB.xlsx
+++ b/kicad/robot/nextPCB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="244">
   <si>
     <t xml:space="preserve">Manufacturer Part Number</t>
   </si>
@@ -61,36 +61,36 @@
     <t xml:space="preserve">GRM155R61E105KA12D</t>
   </si>
   <si>
-    <t xml:space="preserve">C4;C8;C10;C21;C22;C29;C47;C48;C50;C51;C52;C53;C54;C55;C69;C88;C94;C95;C105;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL05A104KA5NNNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C5;C6;C7;C9;C11;C12;C13;C14;C15;C16;C24;C32;C35;C36;C37;C38;C39;C40;C41;C44;C57;C58;C59;C60;C61;C62;C63;C64;C65;C66;C70;C71;C72;C73;C85;C92;C102;C103;C104;</t>
+    <t xml:space="preserve">C4;C8;C10;C21;C22;C29;C47;C48;C50;C51;C52;C53;C54;C55;C69;C88;C94;C95;C105;C126;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM155R62A104KE14D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5;C6;C7;C9;C11;C12;C13;C14;C15;C16;C24;C32;C35;C36;C37;C38;C39;C40;C41;C44;C57;C58;C59;C60;C61;C62;C63;C64;C65;C66;C70;C71;C72;C73;C85;C92;C102;C103;C104;C113;C114;C116;C119;C121;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM188R61E106KA73J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17;C20;C25;C27;C42;C43;C67;C68;C75;C77;C80;C129;C130;C132;C134;C136;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM188R61E475KE11D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23;C97;C100;C101;C124;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL10B474KO8NNNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26;C56;</t>
   </si>
   <si>
     <t xml:space="preserve">Samsung</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM188R61E106KA73J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17;C20;C25;C27;C42;C43;C67;C68;C75;C77;C80;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL21A475KAQNNNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C23;C97;C100;C101;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL10B474KO8NNNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C26;C56;</t>
-  </si>
-  <si>
     <t xml:space="preserve">CL10A225KP8NNNC</t>
   </si>
   <si>
@@ -115,13 +115,46 @@
     <t xml:space="preserve">GRM31CD80J107MEA8K</t>
   </si>
   <si>
-    <t xml:space="preserve">C82;C83;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL05B103KA5NNNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C84;</t>
+    <t xml:space="preserve">C82;C83;C109;C125;C127;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C84;C115;C118;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Würth Elektronik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM155R71H223KA12J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C110;C117;C120;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCM155R71H152KA37D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C111;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCM155R71H332KA37J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C112;C122;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM155R71H473KE14D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C123;C128;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMC32X5R107M16NT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C131;C137;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cal-Chip Electronics, Inc.</t>
   </si>
   <si>
     <t xml:space="preserve">B12H1USD-20D000234U1930</t>
@@ -148,6 +181,18 @@
     <t xml:space="preserve">D3;</t>
   </si>
   <si>
+    <t xml:space="preserve">SMF13A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4;D6;D10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zener diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Littelfuse Inc.</t>
+  </si>
+  <si>
     <t xml:space="preserve">B12H1NG--20D000134U1930</t>
   </si>
   <si>
@@ -163,6 +208,18 @@
     <t xml:space="preserve">KYOCERA AVX</t>
   </si>
   <si>
+    <t xml:space="preserve">1N4448HLP-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D9;D11;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diodes Incorporated</t>
+  </si>
+  <si>
     <t xml:space="preserve">TPS22998RYZR</t>
   </si>
   <si>
@@ -217,6 +274,15 @@
     <t xml:space="preserve">GCT</t>
   </si>
   <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J8;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
     <t xml:space="preserve">NRS6028T1R5NMGJ</t>
   </si>
   <si>
@@ -334,7 +400,7 @@
     <t xml:space="preserve">WR06X1003FTL</t>
   </si>
   <si>
-    <t xml:space="preserve">R12;R17;R49;R59;R60;R61;</t>
+    <t xml:space="preserve">R12;R17;R49;R59;R60;R61;R89;R99;</t>
   </si>
   <si>
     <t xml:space="preserve">Walsin Technology</t>
@@ -367,7 +433,7 @@
     <t xml:space="preserve">WR06X1002FTL</t>
   </si>
   <si>
-    <t xml:space="preserve">R28;R31;</t>
+    <t xml:space="preserve">R28;R31;R96;R102;</t>
   </si>
   <si>
     <t xml:space="preserve">ERJ-3RQJR39V</t>
@@ -379,7 +445,7 @@
     <t xml:space="preserve">Panasonic</t>
   </si>
   <si>
-    <t xml:space="preserve">RMCF0603FT649K</t>
+    <t xml:space="preserve">ERJ-3EKF6493V</t>
   </si>
   <si>
     <t xml:space="preserve">R37;R39;</t>
@@ -391,13 +457,10 @@
     <t xml:space="preserve">R38;R40;</t>
   </si>
   <si>
-    <t xml:space="preserve">ERJ-PA3F2000V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R43;R45;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panasonic Electronic Components</t>
+    <t xml:space="preserve">ERJ-PA3J201V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R43;R45;R103;R104;</t>
   </si>
   <si>
     <t xml:space="preserve">PA0805FRF470R005L</t>
@@ -457,6 +520,27 @@
     <t xml:space="preserve">R95;</t>
   </si>
   <si>
+    <t xml:space="preserve">RC0402FR-13150KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R98;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAGEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-07220KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R100;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-136K8L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R101;</t>
+  </si>
+  <si>
     <t xml:space="preserve">PTS815 SJM 250 SMTR LFS</t>
   </si>
   <si>
@@ -487,10 +571,19 @@
     <t xml:space="preserve">Molex</t>
   </si>
   <si>
+    <t xml:space="preserve">NCU15WF104J6SRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH2;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature dependent resistor</t>
+  </si>
+  <si>
     <t xml:space="preserve">RCUCTE</t>
   </si>
   <si>
-    <t xml:space="preserve">TP1;TP2;TP3;TP4;TP5;TP6;TP7;TP8;TP9;TP11;TP13;TP14;TP15;TP16;TP17;TP18;TP19;TP20;TP21;TP22;TP23;TP24;TP25;TP26;TP27;TP31;TP32;TP33;</t>
+    <t xml:space="preserve">TP1;TP2;TP3;TP4;TP5;TP6;TP7;TP8;TP9;TP10;TP11;TP13;TP14;TP15;TP16;TP17;TP18;TP19;TP20;TP21;TP22;TP23;TP24;TP26;TP27;TP33;</t>
   </si>
   <si>
     <t xml:space="preserve">test point</t>
@@ -505,6 +598,18 @@
     <t xml:space="preserve">Keystone Electronics</t>
   </si>
   <si>
+    <t xml:space="preserve">STWLC38JRM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qi-compliant inductive wireless power receiver for 15W applications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STMicroelectronics</t>
+  </si>
+  <si>
     <t xml:space="preserve">W25Q128JVSIQ</t>
   </si>
   <si>
@@ -569,12 +674,6 @@
   </si>
   <si>
     <t xml:space="preserve">DC Motor Driver I2C Control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM03B-PASS-1-TFT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U10;</t>
   </si>
   <si>
     <t xml:space="preserve">MAX77958EWV+T</t>
@@ -748,7 +847,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -759,7 +858,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="146.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="169.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="103.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.11"/>
@@ -839,7 +938,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>13</v>
@@ -862,7 +961,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>15</v>
@@ -874,7 +973,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,13 +981,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
@@ -905,13 +1004,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>20</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0</v>
@@ -920,7 +1019,7 @@
         <v>8</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,13 +1027,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0</v>
@@ -943,7 +1042,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,7 +1065,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,7 +1122,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>31</v>
@@ -1042,14 +1141,14 @@
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="0" t="n">
+        <v>885012205067</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0</v>
@@ -1058,7 +1157,7 @@
         <v>8</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,7 +1168,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>35</v>
@@ -1078,10 +1177,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,22 +1188,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,22 +1211,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,22 +1234,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,19 +1257,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,22 +1280,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="G19" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,19 +1303,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F20" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="G20" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,22 +1326,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,22 +1349,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1267,19 +1372,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F23" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="G23" s="0" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,22 +1395,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="G24" s="0" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,22 +1415,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1333,22 +1438,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,22 +1461,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F27" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="G27" s="0" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,22 +1481,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1402,22 +1504,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1425,22 +1527,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="G30" s="0" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1448,22 +1547,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,13 +1570,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>0</v>
@@ -1486,7 +1585,7 @@
         <v>89</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1494,22 +1593,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1517,22 +1616,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,22 +1639,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,19 +1662,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D36" s="0" t="s">
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>105</v>
@@ -1589,7 +1688,7 @@
         <v>106</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>107</v>
@@ -1598,10 +1697,10 @@
         <v>0</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,22 +1708,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,22 +1731,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D39" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="G39" s="0" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,22 +1754,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,22 +1777,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,22 +1800,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,22 +1823,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,22 +1846,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,22 +1869,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1793,22 +1892,22 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,22 +1915,22 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,22 +1938,22 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,22 +1961,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1885,22 +1984,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,22 +2007,22 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,22 +2030,22 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,22 +2053,22 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G53" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="C53" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,22 +2076,22 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,22 +2099,22 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,22 +2122,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,45 +2145,45 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="0" t="n">
-        <v>533980271</v>
+      <c r="B58" s="0" t="s">
+        <v>155</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,45 +2191,45 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="0" t="n">
-        <v>5002</v>
+      <c r="B60" s="0" t="s">
+        <v>159</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>160</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2141,7 +2240,7 @@
         <v>161</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>162</v>
@@ -2150,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>164</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,19 +2260,22 @@
         <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F62" s="0" t="s">
+        <v>111</v>
+      </c>
       <c r="G62" s="0" t="s">
-        <v>167</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2181,19 +2283,22 @@
         <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F63" s="0" t="s">
+        <v>111</v>
+      </c>
       <c r="G63" s="0" t="s">
-        <v>170</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,22 +2306,22 @@
         <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>173</v>
+        <v>111</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,19 +2329,22 @@
         <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F65" s="0" t="s">
+        <v>111</v>
+      </c>
       <c r="G65" s="0" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2244,19 +2352,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F66" s="0" t="s">
+        <v>111</v>
+      </c>
       <c r="G66" s="0" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,22 +2375,22 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,42 +2398,45 @@
         <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F68" s="0" t="s">
+        <v>179</v>
+      </c>
       <c r="G68" s="0" t="s">
-        <v>61</v>
+        <v>176</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="0" t="s">
-        <v>185</v>
+      <c r="B69" s="0" t="n">
+        <v>533980271</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,22 +2444,22 @@
         <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,42 +2467,45 @@
         <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F71" s="0" t="s">
+        <v>188</v>
+      </c>
       <c r="G71" s="0" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="0" t="s">
-        <v>192</v>
+      <c r="B72" s="0" t="n">
+        <v>5002</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,19 +2513,22 @@
         <v>72</v>
       </c>
       <c r="B73" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="C73" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D73" s="0" t="s">
+      <c r="G73" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="E73" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G73" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,8 +2547,11 @@
       <c r="E74" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F74" s="0" t="s">
+        <v>198</v>
+      </c>
       <c r="G74" s="0" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,22 +2559,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F75" s="0" t="s">
-        <v>200</v>
-      </c>
       <c r="G75" s="0" t="s">
-        <v>50</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,22 +2579,19 @@
         <v>75</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F76" s="0" t="s">
-        <v>203</v>
-      </c>
       <c r="G76" s="0" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,22 +2599,22 @@
         <v>76</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,22 +2622,283 @@
         <v>77</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F78" s="0" t="s">
-        <v>209</v>
-      </c>
       <c r="G78" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>